<commit_message>
what I believe our basic models will look like. May want to add specific getById queries
</commit_message>
<xml_diff>
--- a/documentation/database.xlsx
+++ b/documentation/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vazqu\Documents\Stevens\Assignments\CS554-Final-Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC94A3C4-06B4-4B11-BC5E-09E647AE1E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B046A4-20A5-4573-9E01-FCAA2E852E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28620" yWindow="-7020" windowWidth="23610" windowHeight="14325" xr2:uid="{034585D4-BB4A-485E-8E08-09671E7B3079}"/>
+    <workbookView xWindow="-22065" yWindow="-6780" windowWidth="19785" windowHeight="15345" activeTab="2" xr2:uid="{034585D4-BB4A-485E-8E08-09671E7B3079}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>field</t>
   </si>
@@ -85,10 +85,13 @@
     <t>USER</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>https://tpiros.dev/blog/image-management-via-graphql/</t>
   </si>
 </sst>
 </file>
@@ -462,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF27587-D8F0-46CC-9C3B-6F407F52EFE2}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +509,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -514,7 +517,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -527,10 +530,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC233E7-30BE-4595-8568-197A9494EB6E}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,6 +579,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -585,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768E164E-7DC9-4830-A1DB-1D04C97D56B2}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>